<commit_message>
Fixed size issue in Div function in SuperInt
</commit_message>
<xml_diff>
--- a/SymbolRecognition/Book1.xlsx
+++ b/SymbolRecognition/Book1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CPPDEV\Projects\CppTests\Tests\Tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CPPDEV\Projects\SymbolRecognition\SymbolRecognition\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1642F040-2CC3-4CD6-98BD-584236760982}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFAF375A-298F-47F8-9EE6-B0342A116C5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1AEA8BA8-B4CB-448A-AEFD-31E17D946A17}"/>
   </bookViews>
@@ -395,10 +395,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6645CEB1-5906-4B60-B0D5-53BF452DFACE}">
-  <dimension ref="A1:T99"/>
+  <dimension ref="A1:T142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
-      <selection activeCell="O77" sqref="O77:S79"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K111" sqref="K111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -406,12 +406,11 @@
     <col min="1" max="8" width="2.77734375" style="1" customWidth="1"/>
     <col min="9" max="9" width="39.6640625" style="1" customWidth="1"/>
     <col min="10" max="10" width="34.5546875" style="1" customWidth="1"/>
-    <col min="11" max="19" width="2.77734375" style="1" customWidth="1"/>
-    <col min="20" max="20" width="25.109375" style="1" customWidth="1"/>
+    <col min="11" max="20" width="2.77734375" style="1" customWidth="1"/>
     <col min="21" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A1" s="1">
         <v>1</v>
       </c>
@@ -419,7 +418,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B2" s="1">
         <v>1</v>
       </c>
@@ -427,103 +426,136 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="C3" s="1">
         <v>1</v>
       </c>
-      <c r="K3" s="1">
-        <v>1</v>
-      </c>
-      <c r="L3" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="M3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="D4" s="1">
         <v>1</v>
       </c>
-      <c r="K4" s="1">
-        <v>1</v>
-      </c>
-      <c r="M4" s="1">
-        <v>1</v>
-      </c>
-      <c r="S4" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="N4" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="E5" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="O5" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="F6" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="P6" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="G7" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="Q7" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="H8" s="1">
         <v>1</v>
       </c>
       <c r="I8" s="1">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="R8" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>1</v>
       </c>
       <c r="B9" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="S9" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>1</v>
       </c>
       <c r="C10" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T10" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>1</v>
       </c>
       <c r="D11" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="K11" s="1">
+        <v>1</v>
+      </c>
+      <c r="L11" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>1</v>
       </c>
       <c r="E12" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="K12" s="1">
+        <v>1</v>
+      </c>
+      <c r="M12" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>1</v>
       </c>
       <c r="F13" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="K13" s="1">
+        <v>1</v>
+      </c>
+      <c r="N13" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>1</v>
       </c>
       <c r="G14" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="K14" s="1">
+        <v>1</v>
+      </c>
+      <c r="O14" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>1</v>
       </c>
@@ -533,32 +565,56 @@
       <c r="I15" s="1">
         <v>7</v>
       </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="K15" s="1">
+        <v>1</v>
+      </c>
+      <c r="P15" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B16" s="1">
         <v>1</v>
       </c>
       <c r="C16" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="K16" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q16" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B17" s="1">
         <v>1</v>
       </c>
       <c r="D17" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="K17" s="1">
+        <v>1</v>
+      </c>
+      <c r="R17" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B18" s="1">
         <v>1</v>
       </c>
       <c r="E18" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="K18" s="1">
+        <v>1</v>
+      </c>
+      <c r="S18" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B19" s="1">
         <v>1</v>
       </c>
@@ -569,21 +625,27 @@
         <v>8</v>
       </c>
       <c r="K19" s="1">
-        <v>7</v>
-      </c>
-      <c r="L19" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="T19" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B20" s="1">
         <v>1</v>
       </c>
       <c r="G20" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="L20" s="1">
+        <v>1</v>
+      </c>
+      <c r="M20" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B21" s="1">
         <v>1</v>
       </c>
@@ -593,40 +655,70 @@
       <c r="I21" s="1">
         <v>6</v>
       </c>
-    </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="L21" s="1">
+        <v>1</v>
+      </c>
+      <c r="N21" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="2:20" x14ac:dyDescent="0.3">
       <c r="C22" s="1">
         <v>1</v>
       </c>
       <c r="D22" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="L22" s="1">
+        <v>1</v>
+      </c>
+      <c r="O22" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="2:20" x14ac:dyDescent="0.3">
       <c r="C23" s="1">
         <v>1</v>
       </c>
       <c r="E23" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="L23" s="1">
+        <v>1</v>
+      </c>
+      <c r="P23" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="2:20" x14ac:dyDescent="0.3">
       <c r="C24" s="1">
         <v>1</v>
       </c>
       <c r="F24" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="L24" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q24" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="2:20" x14ac:dyDescent="0.3">
       <c r="C25" s="1">
         <v>1</v>
       </c>
       <c r="G25" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="L25" s="1">
+        <v>1</v>
+      </c>
+      <c r="R25" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="2:20" x14ac:dyDescent="0.3">
       <c r="C26" s="1">
         <v>1</v>
       </c>
@@ -636,32 +728,56 @@
       <c r="I26" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="L26" s="1">
+        <v>1</v>
+      </c>
+      <c r="S26" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="2:20" x14ac:dyDescent="0.3">
       <c r="D27" s="1">
         <v>1</v>
       </c>
       <c r="E27" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="L27" s="1">
+        <v>1</v>
+      </c>
+      <c r="T27" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="2:20" x14ac:dyDescent="0.3">
       <c r="D28" s="1">
         <v>1</v>
       </c>
       <c r="F28" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M28" s="1">
+        <v>1</v>
+      </c>
+      <c r="N28" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="2:20" x14ac:dyDescent="0.3">
       <c r="D29" s="1">
         <v>1</v>
       </c>
       <c r="G29" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M29" s="1">
+        <v>1</v>
+      </c>
+      <c r="O29" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="2:20" x14ac:dyDescent="0.3">
       <c r="D30" s="1">
         <v>1</v>
       </c>
@@ -671,20 +787,38 @@
       <c r="I30" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="31" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M30" s="1">
+        <v>1</v>
+      </c>
+      <c r="P30" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="2:20" x14ac:dyDescent="0.3">
       <c r="E31" s="1">
         <v>1</v>
       </c>
       <c r="F31" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M31" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q31" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="2:20" x14ac:dyDescent="0.3">
       <c r="E32" s="1">
         <v>1</v>
       </c>
       <c r="G32" s="1">
+        <v>1</v>
+      </c>
+      <c r="M32" s="1">
+        <v>1</v>
+      </c>
+      <c r="R32" s="1">
         <v>1</v>
       </c>
     </row>
@@ -698,6 +832,12 @@
       <c r="I33" s="1">
         <v>3</v>
       </c>
+      <c r="M33" s="1">
+        <v>1</v>
+      </c>
+      <c r="S33" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="34" spans="1:20" x14ac:dyDescent="0.3">
       <c r="F34" s="1">
@@ -706,6 +846,12 @@
       <c r="G34" s="1">
         <v>1</v>
       </c>
+      <c r="M34" s="1">
+        <v>1</v>
+      </c>
+      <c r="T34" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="35" spans="1:20" x14ac:dyDescent="0.3">
       <c r="F35" s="1">
@@ -717,6 +863,12 @@
       <c r="I35" s="1">
         <v>2</v>
       </c>
+      <c r="N35" s="1">
+        <v>1</v>
+      </c>
+      <c r="O35" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="36" spans="1:20" x14ac:dyDescent="0.3">
       <c r="G36" s="1">
@@ -728,6 +880,12 @@
       <c r="I36" s="1">
         <v>1</v>
       </c>
+      <c r="N36" s="1">
+        <v>1</v>
+      </c>
+      <c r="P36" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="37" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
@@ -739,6 +897,12 @@
       <c r="C37" s="1">
         <v>1</v>
       </c>
+      <c r="N37" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q37" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="38" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
@@ -750,6 +914,12 @@
       <c r="D38" s="1">
         <v>1</v>
       </c>
+      <c r="N38" s="1">
+        <v>1</v>
+      </c>
+      <c r="R38" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="39" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
@@ -761,6 +931,12 @@
       <c r="E39" s="1">
         <v>1</v>
       </c>
+      <c r="N39" s="1">
+        <v>1</v>
+      </c>
+      <c r="S39" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="40" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
@@ -772,6 +948,12 @@
       <c r="F40" s="1">
         <v>1</v>
       </c>
+      <c r="N40" s="1">
+        <v>1</v>
+      </c>
+      <c r="T40" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="41" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
@@ -783,6 +965,12 @@
       <c r="G41" s="1">
         <v>1</v>
       </c>
+      <c r="O41" s="1">
+        <v>1</v>
+      </c>
+      <c r="P41" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="42" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
@@ -797,6 +985,12 @@
       <c r="I42" s="1">
         <v>6</v>
       </c>
+      <c r="O42" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q42" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="43" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
@@ -808,6 +1002,12 @@
       <c r="D43" s="1">
         <v>1</v>
       </c>
+      <c r="O43" s="1">
+        <v>1</v>
+      </c>
+      <c r="R43" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="44" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
@@ -819,6 +1019,12 @@
       <c r="E44" s="1">
         <v>1</v>
       </c>
+      <c r="O44" s="1">
+        <v>1</v>
+      </c>
+      <c r="S44" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="45" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
@@ -830,6 +1036,12 @@
       <c r="F45" s="1">
         <v>1</v>
       </c>
+      <c r="O45" s="1">
+        <v>1</v>
+      </c>
+      <c r="T45" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="46" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
@@ -841,7 +1053,7 @@
       <c r="G46" s="1">
         <v>1</v>
       </c>
-      <c r="M46" s="1">
+      <c r="P46" s="1">
         <v>1</v>
       </c>
       <c r="Q46" s="1">
@@ -861,20 +1073,11 @@
       <c r="I47" s="1">
         <v>5</v>
       </c>
-      <c r="L47" s="1">
-        <v>1</v>
-      </c>
-      <c r="N47" s="1">
-        <v>1</v>
-      </c>
       <c r="P47" s="1">
         <v>1</v>
       </c>
       <c r="R47" s="1">
         <v>1</v>
-      </c>
-      <c r="T47" s="1">
-        <v>1.14124124121421E+20</v>
       </c>
     </row>
     <row r="48" spans="1:20" x14ac:dyDescent="0.3">
@@ -887,17 +1090,14 @@
       <c r="E48" s="1">
         <v>1</v>
       </c>
-      <c r="K48" s="1">
-        <v>1</v>
-      </c>
-      <c r="O48" s="1">
+      <c r="P48" s="1">
         <v>1</v>
       </c>
       <c r="S48" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <v>1</v>
       </c>
@@ -907,14 +1107,14 @@
       <c r="F49" s="1">
         <v>1</v>
       </c>
-      <c r="K49" s="1">
-        <v>1</v>
-      </c>
-      <c r="S49" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="P49" s="1">
+        <v>1</v>
+      </c>
+      <c r="T49" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
         <v>1</v>
       </c>
@@ -924,14 +1124,14 @@
       <c r="G50" s="1">
         <v>1</v>
       </c>
-      <c r="L50" s="1">
+      <c r="Q50" s="1">
         <v>1</v>
       </c>
       <c r="R50" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
         <v>1</v>
       </c>
@@ -944,14 +1144,14 @@
       <c r="I51" s="1">
         <v>4</v>
       </c>
-      <c r="M51" s="1">
-        <v>1</v>
-      </c>
       <c r="Q51" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="S51" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
         <v>1</v>
       </c>
@@ -961,14 +1161,14 @@
       <c r="F52" s="1">
         <v>1</v>
       </c>
-      <c r="N52" s="1">
-        <v>1</v>
-      </c>
-      <c r="P52" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="Q52" s="1">
+        <v>1</v>
+      </c>
+      <c r="T52" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A53" s="1">
         <v>1</v>
       </c>
@@ -978,11 +1178,14 @@
       <c r="G53" s="1">
         <v>1</v>
       </c>
+      <c r="R53" s="1">
+        <v>1</v>
+      </c>
       <c r="S53" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A54" s="1">
         <v>1</v>
       </c>
@@ -995,8 +1198,14 @@
       <c r="I54" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="R54" s="1">
+        <v>1</v>
+      </c>
+      <c r="T54" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A55" s="1">
         <v>1</v>
       </c>
@@ -1006,8 +1215,14 @@
       <c r="G55" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="S55" s="1">
+        <v>1</v>
+      </c>
+      <c r="T55" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A56" s="1">
         <v>1</v>
       </c>
@@ -1020,8 +1235,17 @@
       <c r="I56" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="57" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="K56" s="1">
+        <v>1</v>
+      </c>
+      <c r="L56" s="1">
+        <v>1</v>
+      </c>
+      <c r="M56" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A57" s="1">
         <v>1</v>
       </c>
@@ -1034,8 +1258,17 @@
       <c r="I57" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="58" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="K57" s="1">
+        <v>1</v>
+      </c>
+      <c r="L57" s="1">
+        <v>1</v>
+      </c>
+      <c r="N57" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B58" s="1">
         <v>1</v>
       </c>
@@ -1045,8 +1278,17 @@
       <c r="D58" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="59" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="K58" s="1">
+        <v>1</v>
+      </c>
+      <c r="L58" s="1">
+        <v>1</v>
+      </c>
+      <c r="O58" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B59" s="1">
         <v>1</v>
       </c>
@@ -1059,8 +1301,17 @@
       <c r="J59" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="60" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="K59" s="1">
+        <v>1</v>
+      </c>
+      <c r="L59" s="1">
+        <v>1</v>
+      </c>
+      <c r="P59" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B60" s="1">
         <v>1</v>
       </c>
@@ -1070,8 +1321,17 @@
       <c r="F60" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="61" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="K60" s="1">
+        <v>1</v>
+      </c>
+      <c r="L60" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q60" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B61" s="1">
         <v>1</v>
       </c>
@@ -1081,8 +1341,17 @@
       <c r="G61" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="62" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="K61" s="1">
+        <v>1</v>
+      </c>
+      <c r="L61" s="1">
+        <v>1</v>
+      </c>
+      <c r="R61" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B62" s="1">
         <v>1</v>
       </c>
@@ -1095,8 +1364,17 @@
       <c r="I62" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="63" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="K62" s="1">
+        <v>1</v>
+      </c>
+      <c r="L62" s="1">
+        <v>1</v>
+      </c>
+      <c r="S62" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B63" s="1">
         <v>1</v>
       </c>
@@ -1106,8 +1384,17 @@
       <c r="E63" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="64" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="K63" s="1">
+        <v>1</v>
+      </c>
+      <c r="L63" s="1">
+        <v>1</v>
+      </c>
+      <c r="T63" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B64" s="1">
         <v>1</v>
       </c>
@@ -1115,6 +1402,15 @@
         <v>1</v>
       </c>
       <c r="F64" s="1">
+        <v>1</v>
+      </c>
+      <c r="K64" s="1">
+        <v>1</v>
+      </c>
+      <c r="M64" s="1">
+        <v>1</v>
+      </c>
+      <c r="N64" s="1">
         <v>1</v>
       </c>
     </row>
@@ -1128,6 +1424,15 @@
       <c r="G65" s="1">
         <v>1</v>
       </c>
+      <c r="K65" s="1">
+        <v>1</v>
+      </c>
+      <c r="M65" s="1">
+        <v>1</v>
+      </c>
+      <c r="O65" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="66" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B66" s="1">
@@ -1142,6 +1447,15 @@
       <c r="I66" s="1">
         <v>4</v>
       </c>
+      <c r="K66" s="1">
+        <v>1</v>
+      </c>
+      <c r="M66" s="1">
+        <v>1</v>
+      </c>
+      <c r="P66" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="67" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B67" s="1">
@@ -1153,6 +1467,15 @@
       <c r="F67" s="1">
         <v>1</v>
       </c>
+      <c r="K67" s="1">
+        <v>1</v>
+      </c>
+      <c r="M67" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q67" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="68" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B68" s="1">
@@ -1164,6 +1487,15 @@
       <c r="G68" s="1">
         <v>1</v>
       </c>
+      <c r="K68" s="1">
+        <v>1</v>
+      </c>
+      <c r="M68" s="1">
+        <v>1</v>
+      </c>
+      <c r="R68" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="69" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B69" s="1">
@@ -1178,6 +1510,15 @@
       <c r="I69" s="1">
         <v>3</v>
       </c>
+      <c r="K69" s="1">
+        <v>1</v>
+      </c>
+      <c r="M69" s="1">
+        <v>1</v>
+      </c>
+      <c r="S69" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="70" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B70" s="1">
@@ -1189,6 +1530,15 @@
       <c r="G70" s="1">
         <v>1</v>
       </c>
+      <c r="K70" s="1">
+        <v>1</v>
+      </c>
+      <c r="M70" s="1">
+        <v>1</v>
+      </c>
+      <c r="T70" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="71" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B71" s="1">
@@ -1203,6 +1553,15 @@
       <c r="I71" s="1">
         <v>2</v>
       </c>
+      <c r="K71" s="1">
+        <v>1</v>
+      </c>
+      <c r="N71" s="1">
+        <v>1</v>
+      </c>
+      <c r="O71" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="72" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B72" s="1">
@@ -1217,6 +1576,15 @@
       <c r="I72" s="1">
         <v>1</v>
       </c>
+      <c r="K72" s="1">
+        <v>1</v>
+      </c>
+      <c r="N72" s="1">
+        <v>1</v>
+      </c>
+      <c r="P72" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="73" spans="2:20" x14ac:dyDescent="0.3">
       <c r="C73" s="1">
@@ -1231,6 +1599,15 @@
       <c r="J73" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="K73" s="1">
+        <v>1</v>
+      </c>
+      <c r="N73" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q73" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="74" spans="2:20" x14ac:dyDescent="0.3">
       <c r="C74" s="1">
@@ -1242,6 +1619,15 @@
       <c r="F74" s="1">
         <v>1</v>
       </c>
+      <c r="K74" s="1">
+        <v>1</v>
+      </c>
+      <c r="N74" s="1">
+        <v>1</v>
+      </c>
+      <c r="R74" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="75" spans="2:20" x14ac:dyDescent="0.3">
       <c r="C75" s="1">
@@ -1253,6 +1639,15 @@
       <c r="G75" s="1">
         <v>1</v>
       </c>
+      <c r="K75" s="1">
+        <v>1</v>
+      </c>
+      <c r="N75" s="1">
+        <v>1</v>
+      </c>
+      <c r="S75" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="76" spans="2:20" x14ac:dyDescent="0.3">
       <c r="C76" s="1">
@@ -1267,6 +1662,15 @@
       <c r="I76" s="1">
         <v>4</v>
       </c>
+      <c r="K76" s="1">
+        <v>1</v>
+      </c>
+      <c r="N76" s="1">
+        <v>1</v>
+      </c>
+      <c r="T76" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="77" spans="2:20" x14ac:dyDescent="0.3">
       <c r="C77" s="1">
@@ -1278,23 +1682,14 @@
       <c r="F77" s="1">
         <v>1</v>
       </c>
+      <c r="K77" s="1">
+        <v>1</v>
+      </c>
       <c r="O77" s="1">
         <v>1</v>
       </c>
       <c r="P77" s="1">
         <v>1</v>
-      </c>
-      <c r="Q77" s="1">
-        <v>0</v>
-      </c>
-      <c r="R77" s="1">
-        <v>1</v>
-      </c>
-      <c r="S77" s="1">
-        <v>1</v>
-      </c>
-      <c r="T77" s="1">
-        <v>18</v>
       </c>
     </row>
     <row r="78" spans="2:20" x14ac:dyDescent="0.3">
@@ -1307,20 +1702,14 @@
       <c r="G78" s="1">
         <v>1</v>
       </c>
+      <c r="K78" s="1">
+        <v>1</v>
+      </c>
       <c r="O78" s="1">
-        <v>0</v>
-      </c>
-      <c r="P78" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q78" s="1">
         <v>1</v>
-      </c>
-      <c r="R78" s="1">
-        <v>1</v>
-      </c>
-      <c r="S78" s="1">
-        <v>0</v>
       </c>
     </row>
     <row r="79" spans="2:20" x14ac:dyDescent="0.3">
@@ -1336,19 +1725,13 @@
       <c r="I79" s="1">
         <v>3</v>
       </c>
+      <c r="K79" s="1">
+        <v>1</v>
+      </c>
       <c r="O79" s="1">
         <v>1</v>
       </c>
-      <c r="P79" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q79" s="1">
-        <v>1</v>
-      </c>
       <c r="R79" s="1">
-        <v>0</v>
-      </c>
-      <c r="S79" s="1">
         <v>1</v>
       </c>
     </row>
@@ -1362,8 +1745,17 @@
       <c r="G80" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K80" s="1">
+        <v>1</v>
+      </c>
+      <c r="O80" s="1">
+        <v>1</v>
+      </c>
+      <c r="S80" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:20" x14ac:dyDescent="0.3">
       <c r="C81" s="1">
         <v>1</v>
       </c>
@@ -1376,8 +1768,17 @@
       <c r="I81" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K81" s="1">
+        <v>1</v>
+      </c>
+      <c r="O81" s="1">
+        <v>1</v>
+      </c>
+      <c r="T81" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:20" x14ac:dyDescent="0.3">
       <c r="C82" s="1">
         <v>1</v>
       </c>
@@ -1390,8 +1791,17 @@
       <c r="I82" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K82" s="1">
+        <v>1</v>
+      </c>
+      <c r="P82" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q82" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:20" x14ac:dyDescent="0.3">
       <c r="D83" s="1">
         <v>1</v>
       </c>
@@ -1401,8 +1811,17 @@
       <c r="F83" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K83" s="1">
+        <v>1</v>
+      </c>
+      <c r="P83" s="1">
+        <v>1</v>
+      </c>
+      <c r="R83" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:20" x14ac:dyDescent="0.3">
       <c r="D84" s="1">
         <v>1</v>
       </c>
@@ -1412,8 +1831,17 @@
       <c r="G84" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K84" s="1">
+        <v>1</v>
+      </c>
+      <c r="P84" s="1">
+        <v>1</v>
+      </c>
+      <c r="S84" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:20" x14ac:dyDescent="0.3">
       <c r="D85" s="1">
         <v>1</v>
       </c>
@@ -1426,8 +1854,17 @@
       <c r="I85" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K85" s="1">
+        <v>1</v>
+      </c>
+      <c r="P85" s="1">
+        <v>1</v>
+      </c>
+      <c r="T85" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:20" x14ac:dyDescent="0.3">
       <c r="D86" s="1">
         <v>1</v>
       </c>
@@ -1437,8 +1874,17 @@
       <c r="G86" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K86" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q86" s="1">
+        <v>1</v>
+      </c>
+      <c r="R86" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:20" x14ac:dyDescent="0.3">
       <c r="D87" s="1">
         <v>1</v>
       </c>
@@ -1451,8 +1897,17 @@
       <c r="I87" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K87" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q87" s="1">
+        <v>1</v>
+      </c>
+      <c r="S87" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:20" x14ac:dyDescent="0.3">
       <c r="D88" s="1">
         <v>1</v>
       </c>
@@ -1465,8 +1920,17 @@
       <c r="I88" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K88" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q88" s="1">
+        <v>1</v>
+      </c>
+      <c r="T88" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:20" x14ac:dyDescent="0.3">
       <c r="E89" s="1">
         <v>1</v>
       </c>
@@ -1476,8 +1940,17 @@
       <c r="G89" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K89" s="1">
+        <v>1</v>
+      </c>
+      <c r="R89" s="1">
+        <v>1</v>
+      </c>
+      <c r="S89" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:20" x14ac:dyDescent="0.3">
       <c r="E90" s="1">
         <v>1</v>
       </c>
@@ -1490,8 +1963,17 @@
       <c r="I90" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K90" s="1">
+        <v>1</v>
+      </c>
+      <c r="R90" s="1">
+        <v>1</v>
+      </c>
+      <c r="T90" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:20" x14ac:dyDescent="0.3">
       <c r="E91" s="1">
         <v>1</v>
       </c>
@@ -1504,8 +1986,17 @@
       <c r="I91" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K91" s="1">
+        <v>1</v>
+      </c>
+      <c r="S91" s="1">
+        <v>1</v>
+      </c>
+      <c r="T91" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:20" x14ac:dyDescent="0.3">
       <c r="F92" s="1">
         <v>1</v>
       </c>
@@ -1518,8 +2009,17 @@
       <c r="I92" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L92" s="1">
+        <v>1</v>
+      </c>
+      <c r="M92" s="1">
+        <v>1</v>
+      </c>
+      <c r="N92" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A93" s="1">
         <v>1</v>
       </c>
@@ -1532,8 +2032,17 @@
       <c r="D93" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L93" s="1">
+        <v>1</v>
+      </c>
+      <c r="M93" s="1">
+        <v>1</v>
+      </c>
+      <c r="O93" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A94" s="1">
         <v>1</v>
       </c>
@@ -1546,8 +2055,17 @@
       <c r="E94" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L94" s="1">
+        <v>1</v>
+      </c>
+      <c r="M94" s="1">
+        <v>1</v>
+      </c>
+      <c r="P94" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A95" s="1">
         <v>1</v>
       </c>
@@ -1560,8 +2078,17 @@
       <c r="F95" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L95" s="1">
+        <v>1</v>
+      </c>
+      <c r="M95" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q95" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A96" s="1">
         <v>1</v>
       </c>
@@ -1574,8 +2101,17 @@
       <c r="G96" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L96" s="1">
+        <v>1</v>
+      </c>
+      <c r="M96" s="1">
+        <v>1</v>
+      </c>
+      <c r="R96" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A97" s="1">
         <v>1</v>
       </c>
@@ -1588,8 +2124,17 @@
       <c r="H97" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L97" s="1">
+        <v>1</v>
+      </c>
+      <c r="M97" s="1">
+        <v>1</v>
+      </c>
+      <c r="S97" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A98" s="1">
         <v>1</v>
       </c>
@@ -1602,8 +2147,17 @@
       <c r="E98" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L98" s="1">
+        <v>1</v>
+      </c>
+      <c r="M98" s="1">
+        <v>1</v>
+      </c>
+      <c r="T98" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A99" s="1">
         <v>1</v>
       </c>
@@ -1618,6 +2172,797 @@
       </c>
       <c r="J99" s="1" t="s">
         <v>2</v>
+      </c>
+      <c r="L99" s="1">
+        <v>1</v>
+      </c>
+      <c r="N99" s="1">
+        <v>1</v>
+      </c>
+      <c r="O99" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A100" s="1">
+        <v>1</v>
+      </c>
+      <c r="B100" s="1">
+        <v>1</v>
+      </c>
+      <c r="D100" s="1">
+        <v>1</v>
+      </c>
+      <c r="G100" s="1">
+        <v>1</v>
+      </c>
+      <c r="L100" s="1">
+        <v>1</v>
+      </c>
+      <c r="N100" s="1">
+        <v>1</v>
+      </c>
+      <c r="P100" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A101" s="1">
+        <v>1</v>
+      </c>
+      <c r="B101" s="1">
+        <v>1</v>
+      </c>
+      <c r="D101" s="1">
+        <v>1</v>
+      </c>
+      <c r="H101" s="1">
+        <v>1</v>
+      </c>
+      <c r="L101" s="1">
+        <v>1</v>
+      </c>
+      <c r="N101" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q101" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A102" s="1">
+        <v>1</v>
+      </c>
+      <c r="B102" s="1">
+        <v>1</v>
+      </c>
+      <c r="E102" s="1">
+        <v>1</v>
+      </c>
+      <c r="F102" s="1">
+        <v>1</v>
+      </c>
+      <c r="L102" s="1">
+        <v>1</v>
+      </c>
+      <c r="N102" s="1">
+        <v>1</v>
+      </c>
+      <c r="R102" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A103" s="1">
+        <v>1</v>
+      </c>
+      <c r="B103" s="1">
+        <v>1</v>
+      </c>
+      <c r="E103" s="1">
+        <v>1</v>
+      </c>
+      <c r="G103" s="1">
+        <v>1</v>
+      </c>
+      <c r="L103" s="1">
+        <v>1</v>
+      </c>
+      <c r="N103" s="1">
+        <v>1</v>
+      </c>
+      <c r="S103" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A104" s="1">
+        <v>1</v>
+      </c>
+      <c r="B104" s="1">
+        <v>1</v>
+      </c>
+      <c r="E104" s="1">
+        <v>1</v>
+      </c>
+      <c r="H104" s="1">
+        <v>1</v>
+      </c>
+      <c r="L104" s="1">
+        <v>1</v>
+      </c>
+      <c r="N104" s="1">
+        <v>1</v>
+      </c>
+      <c r="T104" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A105" s="1">
+        <v>1</v>
+      </c>
+      <c r="B105" s="1">
+        <v>1</v>
+      </c>
+      <c r="F105" s="1">
+        <v>1</v>
+      </c>
+      <c r="G105" s="1">
+        <v>1</v>
+      </c>
+      <c r="L105" s="1">
+        <v>1</v>
+      </c>
+      <c r="O105" s="1">
+        <v>1</v>
+      </c>
+      <c r="P105" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A106" s="1">
+        <v>1</v>
+      </c>
+      <c r="B106" s="1">
+        <v>1</v>
+      </c>
+      <c r="F106" s="1">
+        <v>1</v>
+      </c>
+      <c r="H106" s="1">
+        <v>1</v>
+      </c>
+      <c r="L106" s="1">
+        <v>1</v>
+      </c>
+      <c r="O106" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q106" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A107" s="1">
+        <v>1</v>
+      </c>
+      <c r="B107" s="1">
+        <v>1</v>
+      </c>
+      <c r="G107" s="1">
+        <v>1</v>
+      </c>
+      <c r="H107" s="1">
+        <v>1</v>
+      </c>
+      <c r="L107" s="1">
+        <v>1</v>
+      </c>
+      <c r="O107" s="1">
+        <v>1</v>
+      </c>
+      <c r="R107" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A108" s="1">
+        <v>1</v>
+      </c>
+      <c r="C108" s="1">
+        <v>1</v>
+      </c>
+      <c r="D108" s="1">
+        <v>1</v>
+      </c>
+      <c r="E108" s="1">
+        <v>1</v>
+      </c>
+      <c r="L108" s="1">
+        <v>1</v>
+      </c>
+      <c r="O108" s="1">
+        <v>1</v>
+      </c>
+      <c r="S108" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A109" s="1">
+        <v>1</v>
+      </c>
+      <c r="C109" s="1">
+        <v>1</v>
+      </c>
+      <c r="D109" s="1">
+        <v>1</v>
+      </c>
+      <c r="F109" s="1">
+        <v>1</v>
+      </c>
+      <c r="L109" s="1">
+        <v>1</v>
+      </c>
+      <c r="O109" s="1">
+        <v>1</v>
+      </c>
+      <c r="T109" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A110" s="1">
+        <v>1</v>
+      </c>
+      <c r="C110" s="1">
+        <v>1</v>
+      </c>
+      <c r="D110" s="1">
+        <v>1</v>
+      </c>
+      <c r="G110" s="1">
+        <v>1</v>
+      </c>
+      <c r="L110" s="1">
+        <v>1</v>
+      </c>
+      <c r="P110" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q110" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A111" s="1">
+        <v>1</v>
+      </c>
+      <c r="C111" s="1">
+        <v>1</v>
+      </c>
+      <c r="D111" s="1">
+        <v>1</v>
+      </c>
+      <c r="H111" s="1">
+        <v>1</v>
+      </c>
+      <c r="L111" s="1">
+        <v>1</v>
+      </c>
+      <c r="P111" s="1">
+        <v>1</v>
+      </c>
+      <c r="R111" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A112" s="1">
+        <v>1</v>
+      </c>
+      <c r="C112" s="1">
+        <v>1</v>
+      </c>
+      <c r="E112" s="1">
+        <v>1</v>
+      </c>
+      <c r="F112" s="1">
+        <v>1</v>
+      </c>
+      <c r="L112" s="1">
+        <v>1</v>
+      </c>
+      <c r="P112" s="1">
+        <v>1</v>
+      </c>
+      <c r="S112" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A113" s="1">
+        <v>1</v>
+      </c>
+      <c r="C113" s="1">
+        <v>1</v>
+      </c>
+      <c r="E113" s="1">
+        <v>1</v>
+      </c>
+      <c r="G113" s="1">
+        <v>1</v>
+      </c>
+      <c r="L113" s="1">
+        <v>1</v>
+      </c>
+      <c r="P113" s="1">
+        <v>1</v>
+      </c>
+      <c r="T113" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A114" s="1">
+        <v>1</v>
+      </c>
+      <c r="C114" s="1">
+        <v>1</v>
+      </c>
+      <c r="E114" s="1">
+        <v>1</v>
+      </c>
+      <c r="H114" s="1">
+        <v>1</v>
+      </c>
+      <c r="L114" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q114" s="1">
+        <v>1</v>
+      </c>
+      <c r="R114" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A115" s="1">
+        <v>1</v>
+      </c>
+      <c r="C115" s="1">
+        <v>1</v>
+      </c>
+      <c r="F115" s="1">
+        <v>1</v>
+      </c>
+      <c r="G115" s="1">
+        <v>1</v>
+      </c>
+      <c r="L115" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q115" s="1">
+        <v>1</v>
+      </c>
+      <c r="S115" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A116" s="1">
+        <v>1</v>
+      </c>
+      <c r="C116" s="1">
+        <v>1</v>
+      </c>
+      <c r="F116" s="1">
+        <v>1</v>
+      </c>
+      <c r="H116" s="1">
+        <v>1</v>
+      </c>
+      <c r="L116" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q116" s="1">
+        <v>1</v>
+      </c>
+      <c r="T116" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A117" s="1">
+        <v>1</v>
+      </c>
+      <c r="C117" s="1">
+        <v>1</v>
+      </c>
+      <c r="G117" s="1">
+        <v>1</v>
+      </c>
+      <c r="H117" s="1">
+        <v>1</v>
+      </c>
+      <c r="L117" s="1">
+        <v>1</v>
+      </c>
+      <c r="R117" s="1">
+        <v>1</v>
+      </c>
+      <c r="S117" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A118" s="1">
+        <v>1</v>
+      </c>
+      <c r="D118" s="1">
+        <v>1</v>
+      </c>
+      <c r="E118" s="1">
+        <v>1</v>
+      </c>
+      <c r="F118" s="1">
+        <v>1</v>
+      </c>
+      <c r="L118" s="1">
+        <v>1</v>
+      </c>
+      <c r="R118" s="1">
+        <v>1</v>
+      </c>
+      <c r="T118" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A119" s="1">
+        <v>1</v>
+      </c>
+      <c r="D119" s="1">
+        <v>1</v>
+      </c>
+      <c r="E119" s="1">
+        <v>1</v>
+      </c>
+      <c r="G119" s="1">
+        <v>1</v>
+      </c>
+      <c r="L119" s="1">
+        <v>1</v>
+      </c>
+      <c r="S119" s="1">
+        <v>1</v>
+      </c>
+      <c r="T119" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A120" s="1">
+        <v>1</v>
+      </c>
+      <c r="D120" s="1">
+        <v>1</v>
+      </c>
+      <c r="E120" s="1">
+        <v>1</v>
+      </c>
+      <c r="H120" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A121" s="1">
+        <v>1</v>
+      </c>
+      <c r="D121" s="1">
+        <v>1</v>
+      </c>
+      <c r="F121" s="1">
+        <v>1</v>
+      </c>
+      <c r="G121" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A122" s="1">
+        <v>1</v>
+      </c>
+      <c r="D122" s="1">
+        <v>1</v>
+      </c>
+      <c r="F122" s="1">
+        <v>1</v>
+      </c>
+      <c r="H122" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A123" s="1">
+        <v>1</v>
+      </c>
+      <c r="D123" s="1">
+        <v>1</v>
+      </c>
+      <c r="G123" s="1">
+        <v>1</v>
+      </c>
+      <c r="H123" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="124" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A124" s="1">
+        <v>1</v>
+      </c>
+      <c r="E124" s="1">
+        <v>1</v>
+      </c>
+      <c r="F124" s="1">
+        <v>1</v>
+      </c>
+      <c r="G124" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="125" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A125" s="1">
+        <v>1</v>
+      </c>
+      <c r="E125" s="1">
+        <v>1</v>
+      </c>
+      <c r="F125" s="1">
+        <v>1</v>
+      </c>
+      <c r="H125" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="126" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A126" s="1">
+        <v>1</v>
+      </c>
+      <c r="E126" s="1">
+        <v>1</v>
+      </c>
+      <c r="G126" s="1">
+        <v>1</v>
+      </c>
+      <c r="H126" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="127" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A127" s="1">
+        <v>1</v>
+      </c>
+      <c r="F127" s="1">
+        <v>1</v>
+      </c>
+      <c r="G127" s="1">
+        <v>1</v>
+      </c>
+      <c r="H127" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="128" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="B128" s="1">
+        <v>1</v>
+      </c>
+      <c r="C128" s="1">
+        <v>1</v>
+      </c>
+      <c r="D128" s="1">
+        <v>1</v>
+      </c>
+      <c r="E128" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="129" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B129" s="1">
+        <v>1</v>
+      </c>
+      <c r="C129" s="1">
+        <v>1</v>
+      </c>
+      <c r="D129" s="1">
+        <v>1</v>
+      </c>
+      <c r="F129" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B130" s="1">
+        <v>1</v>
+      </c>
+      <c r="C130" s="1">
+        <v>1</v>
+      </c>
+      <c r="D130" s="1">
+        <v>1</v>
+      </c>
+      <c r="G130" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="131" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B131" s="1">
+        <v>1</v>
+      </c>
+      <c r="C131" s="1">
+        <v>1</v>
+      </c>
+      <c r="D131" s="1">
+        <v>1</v>
+      </c>
+      <c r="H131" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="132" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B132" s="1">
+        <v>1</v>
+      </c>
+      <c r="C132" s="1">
+        <v>1</v>
+      </c>
+      <c r="E132" s="1">
+        <v>1</v>
+      </c>
+      <c r="F132" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B133" s="1">
+        <v>1</v>
+      </c>
+      <c r="C133" s="1">
+        <v>1</v>
+      </c>
+      <c r="E133" s="1">
+        <v>1</v>
+      </c>
+      <c r="G133" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="134" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B134" s="1">
+        <v>1</v>
+      </c>
+      <c r="C134" s="1">
+        <v>1</v>
+      </c>
+      <c r="E134" s="1">
+        <v>1</v>
+      </c>
+      <c r="H134" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B135" s="1">
+        <v>1</v>
+      </c>
+      <c r="C135" s="1">
+        <v>1</v>
+      </c>
+      <c r="F135" s="1">
+        <v>1</v>
+      </c>
+      <c r="G135" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="136" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B136" s="1">
+        <v>1</v>
+      </c>
+      <c r="C136" s="1">
+        <v>1</v>
+      </c>
+      <c r="F136" s="1">
+        <v>1</v>
+      </c>
+      <c r="H136" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="137" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B137" s="1">
+        <v>1</v>
+      </c>
+      <c r="C137" s="1">
+        <v>1</v>
+      </c>
+      <c r="G137" s="1">
+        <v>1</v>
+      </c>
+      <c r="H137" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="138" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B138" s="1">
+        <v>1</v>
+      </c>
+      <c r="D138" s="1">
+        <v>1</v>
+      </c>
+      <c r="E138" s="1">
+        <v>1</v>
+      </c>
+      <c r="F138" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="139" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B139" s="1">
+        <v>1</v>
+      </c>
+      <c r="D139" s="1">
+        <v>1</v>
+      </c>
+      <c r="E139" s="1">
+        <v>1</v>
+      </c>
+      <c r="G139" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="140" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B140" s="1">
+        <v>1</v>
+      </c>
+      <c r="D140" s="1">
+        <v>1</v>
+      </c>
+      <c r="E140" s="1">
+        <v>1</v>
+      </c>
+      <c r="H140" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="141" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B141" s="1">
+        <v>1</v>
+      </c>
+      <c r="D141" s="1">
+        <v>1</v>
+      </c>
+      <c r="F141" s="1">
+        <v>1</v>
+      </c>
+      <c r="G141" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="142" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B142" s="1">
+        <v>1</v>
+      </c>
+      <c r="D142" s="1">
+        <v>1</v>
+      </c>
+      <c r="F142" s="1">
+        <v>1</v>
+      </c>
+      <c r="H142" s="1">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>